<commit_message>
add person_table, update processSheet
</commit_message>
<xml_diff>
--- a/Documents/processSheet.xlsx
+++ b/Documents/processSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="103">
   <si>
     <t>担当</t>
     <rPh sb="0" eb="2">
@@ -640,6 +640,96 @@
     <rPh sb="9" eb="11">
       <t>ケントウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ドキュメント作成</t>
+    <rPh sb="6" eb="8">
+      <t>サクセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ドキュメント</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ui/メインフレーム</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ドキュメント/リファレンス共有</t>
+    <rPh sb="13" eb="15">
+      <t>キョウユウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>澤口</t>
+    <rPh sb="0" eb="2">
+      <t>サワグチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>市名</t>
+    <rPh sb="0" eb="1">
+      <t>イチ</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>ナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>谷口・澤口</t>
+    <rPh sb="0" eb="2">
+      <t>タニグチ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>サワグチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>中野・市名</t>
+    <rPh sb="0" eb="2">
+      <t>ナカノ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>イチ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>澤口・仁木</t>
+    <rPh sb="0" eb="2">
+      <t>サワグチ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ニキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>市名</t>
+    <rPh sb="0" eb="2">
+      <t>イチナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ドキュメント・リファレンス共有</t>
+    <rPh sb="13" eb="15">
+      <t>キョウユウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UI・メインフレーム</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -692,7 +782,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -794,6 +884,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -883,7 +979,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1036,6 +1132,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1365,10 +1464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CN60"/>
+  <dimension ref="A1:CN62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1642,7 +1741,7 @@
       </c>
       <c r="C4" s="35"/>
       <c r="D4" s="21" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="E4" s="31"/>
       <c r="F4" s="32"/>
@@ -1808,7 +1907,9 @@
       <c r="AT7" s="4"/>
     </row>
     <row r="8" spans="1:92" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="7"/>
+      <c r="A8" s="7" t="s">
+        <v>93</v>
+      </c>
       <c r="B8" s="7" t="s">
         <v>79</v>
       </c>
@@ -1853,13 +1954,15 @@
       <c r="CB8" s="4"/>
     </row>
     <row r="9" spans="1:92" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="7"/>
+      <c r="A9" s="7" t="s">
+        <v>94</v>
+      </c>
       <c r="B9" s="7" t="s">
         <v>81</v>
       </c>
       <c r="C9" s="43"/>
       <c r="D9" s="22" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="11"/>
@@ -2112,7 +2215,7 @@
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="22" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E15" s="39"/>
       <c r="F15" s="39"/>
@@ -2186,41 +2289,47 @@
       <c r="AI16" s="11"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="7"/>
-      <c r="Z17" s="7"/>
-      <c r="AA17" s="11"/>
-      <c r="AB17" s="11"/>
-      <c r="AC17" s="7"/>
-      <c r="AD17" s="7"/>
-      <c r="AE17" s="7"/>
-      <c r="AF17" s="7"/>
-      <c r="AG17" s="7"/>
-      <c r="AH17" s="11"/>
-      <c r="AI17" s="11"/>
+      <c r="A17" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="51"/>
+      <c r="D17" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="51"/>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="51"/>
+      <c r="S17" s="51"/>
+      <c r="T17" s="51"/>
+      <c r="U17" s="51"/>
+      <c r="V17" s="51"/>
+      <c r="W17" s="51"/>
+      <c r="X17" s="51"/>
+      <c r="Y17" s="51"/>
+      <c r="Z17" s="51"/>
+      <c r="AA17" s="51"/>
+      <c r="AB17" s="51"/>
+      <c r="AC17" s="51"/>
+      <c r="AD17" s="51"/>
+      <c r="AE17" s="51"/>
+      <c r="AF17" s="51"/>
+      <c r="AG17" s="51"/>
+      <c r="AH17" s="51"/>
+      <c r="AI17" s="51"/>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="7"/>
@@ -2538,7 +2647,7 @@
       </c>
       <c r="C26" s="35"/>
       <c r="D26" s="21" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="19"/>
@@ -2579,7 +2688,7 @@
       </c>
       <c r="C27" s="36"/>
       <c r="D27" s="21" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
@@ -2620,7 +2729,7 @@
       </c>
       <c r="C28" s="37"/>
       <c r="D28" s="22" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="E28" s="37"/>
       <c r="F28" s="37"/>
@@ -2661,7 +2770,7 @@
       </c>
       <c r="C29" s="41"/>
       <c r="D29" s="22" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E29" s="41"/>
       <c r="F29" s="41"/>
@@ -2702,7 +2811,7 @@
       </c>
       <c r="C30" s="40"/>
       <c r="D30" s="22" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E30" s="40"/>
       <c r="F30" s="40"/>
@@ -2743,7 +2852,7 @@
       </c>
       <c r="C31" s="43"/>
       <c r="D31" s="22" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
@@ -2823,7 +2932,7 @@
       </c>
       <c r="C33" s="38"/>
       <c r="D33" s="21" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
@@ -2864,7 +2973,7 @@
       </c>
       <c r="C34" s="42"/>
       <c r="D34" s="21" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="19"/>
@@ -2981,7 +3090,7 @@
       </c>
       <c r="C37" s="39"/>
       <c r="D37" s="22" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="E37" s="24"/>
       <c r="F37" s="24"/>
@@ -3053,41 +3162,47 @@
       <c r="AI38" s="19"/>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="19"/>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="20"/>
-      <c r="R39" s="11"/>
-      <c r="S39" s="19"/>
-      <c r="T39" s="7"/>
-      <c r="U39" s="7"/>
-      <c r="V39" s="19"/>
-      <c r="W39" s="7"/>
-      <c r="X39" s="11"/>
-      <c r="Y39" s="20"/>
-      <c r="Z39" s="7"/>
-      <c r="AA39" s="19"/>
-      <c r="AB39" s="7"/>
-      <c r="AC39" s="19"/>
-      <c r="AD39" s="7"/>
-      <c r="AE39" s="20"/>
-      <c r="AF39" s="11"/>
-      <c r="AG39" s="19"/>
-      <c r="AH39" s="7"/>
-      <c r="AI39" s="19"/>
+      <c r="A39" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="51"/>
+      <c r="D39" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="51"/>
+      <c r="O39" s="51"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="51"/>
+      <c r="R39" s="51"/>
+      <c r="S39" s="51"/>
+      <c r="T39" s="51"/>
+      <c r="U39" s="51"/>
+      <c r="V39" s="51"/>
+      <c r="W39" s="51"/>
+      <c r="X39" s="51"/>
+      <c r="Y39" s="51"/>
+      <c r="Z39" s="51"/>
+      <c r="AA39" s="51"/>
+      <c r="AB39" s="51"/>
+      <c r="AC39" s="51"/>
+      <c r="AD39" s="51"/>
+      <c r="AE39" s="51"/>
+      <c r="AF39" s="51"/>
+      <c r="AG39" s="51"/>
+      <c r="AH39" s="51"/>
+      <c r="AI39" s="51"/>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="7"/>
@@ -3280,6 +3395,22 @@
       </c>
       <c r="C60" s="25"/>
     </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D53:G53"/>

</xml_diff>